<commit_message>
implemented more flows for vacation collection
</commit_message>
<xml_diff>
--- a/doc/vacation-collection/vacation-collection-decision-table.xlsx
+++ b/doc/vacation-collection/vacation-collection-decision-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects.pet\VeloCity\repo\doc\vacation-collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506A116B-1BB4-4B51-936D-28BF554B254D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC0BEBF-26FE-453B-A104-80D8EB9ACEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="3" activeTab="3" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="current is none" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="69">
   <si>
     <t>any</t>
   </si>
@@ -101,12 +101,6 @@
     <t>Results</t>
   </si>
   <si>
-    <t>remove previous and current and extend next to start from previous</t>
-  </si>
-  <si>
-    <t>remove previous and current and create daily from previous to current</t>
-  </si>
-  <si>
     <t>extend previous to end to current</t>
   </si>
   <si>
@@ -119,24 +113,6 @@
     <t>single day</t>
   </si>
   <si>
-    <t>remove previous, current and next and replace with daily from previous to next</t>
-  </si>
-  <si>
-    <t>remove current and next and extend previous to end to next</t>
-  </si>
-  <si>
-    <t>remove current and next and extend previous to end to next's end</t>
-  </si>
-  <si>
-    <t>remove current and extend previous to end to current</t>
-  </si>
-  <si>
-    <t>remove current and next and create daily from current to next</t>
-  </si>
-  <si>
-    <t>remove current and extend next to start from current</t>
-  </si>
-  <si>
     <t>update current hours</t>
   </si>
   <si>
@@ -209,9 +185,6 @@
     <t>update next hours (dangerous because past analysis will be impacted)</t>
   </si>
   <si>
-    <t>remove current and create once</t>
-  </si>
-  <si>
     <t>daily (only for current)</t>
   </si>
   <si>
@@ -221,12 +194,6 @@
     <t>daily (start from previous and goes to next)</t>
   </si>
   <si>
-    <t>update daily to end to previous day, create daily from next to previous's end</t>
-  </si>
-  <si>
-    <t>update daily to end to previous day, create once for current, create daily from next day to previous's end</t>
-  </si>
-  <si>
     <t>update daily vacation hours (dangerous because past analysis will be impacted)</t>
   </si>
   <si>
@@ -245,9 +212,6 @@
     <t>remove next; extend previous to end to the next's end</t>
   </si>
   <si>
-    <t>remove next; extend previous to end to current</t>
-  </si>
-  <si>
     <t>remove next; create daily from current to next</t>
   </si>
   <si>
@@ -272,13 +236,19 @@
     <t>remove current; extend previous to end to current</t>
   </si>
   <si>
-    <t>remove current; next and create daily from current to next</t>
-  </si>
-  <si>
     <t>remove current; extend next to start from current</t>
   </si>
   <si>
     <t>remove current and next; create daily from current to next</t>
+  </si>
+  <si>
+    <t>remove current; create once</t>
+  </si>
+  <si>
+    <t>update current daily to end to previous day; create daily from next to previous' end</t>
+  </si>
+  <si>
+    <t>update current daily to end to previous day; create once for current; create daily from next day to previous' end</t>
   </si>
 </sst>
 </file>
@@ -361,7 +331,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -374,25 +344,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -715,7 +676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7:E9"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,11 +721,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -786,17 +747,17 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -806,15 +767,15 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
@@ -822,15 +783,15 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
@@ -838,14 +799,14 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
@@ -856,235 +817,235 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" t="s">
         <v>0</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7" t="s">
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" t="s">
         <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="C3:C14"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E5"/>
     <mergeCell ref="B3:B18"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="C3:C14"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1097,7 +1058,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,11 +1103,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1168,17 +1129,17 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1188,269 +1149,269 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" t="s">
         <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" t="s">
         <v>0</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" t="s">
         <v>5</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" t="s">
         <v>6</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" t="s">
         <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" t="s">
         <v>4</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" t="s">
         <v>6</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" t="s">
         <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7A479A-DDB0-4158-9294-15531397EDCA}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
@@ -1528,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1543,10 +1504,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1560,7 +1521,7 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,10 +1542,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1598,11 +1559,12 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A5"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
@@ -1613,7 +1575,6 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1624,9 +1585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3876F166-8D3B-406C-AA2F-FB4692170FD0}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,53 +1624,53 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>69</v>
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
@@ -1717,124 +1678,124 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="D5:D7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="D5:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1884,53 +1845,53 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>69</v>
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
@@ -1938,113 +1899,113 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2029,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11:D14"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,11 +2074,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
+      <c r="A2" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2139,294 +2100,294 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" t="s">
         <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" t="s">
         <v>0</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" t="s">
         <v>5</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" t="s">
         <v>6</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" t="s">
         <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" t="s">
         <v>4</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" t="s">
         <v>6</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" t="s">
         <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2455,7 +2416,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,33 +2445,33 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>69</v>
+      <c r="A2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
+      <c r="A4" s="7"/>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2520,25 +2481,25 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3"/>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>